<commit_message>
Map federal states using boundaries-schema
</commit_message>
<xml_diff>
--- a/src/egon/data/importing/nep_input_data/NEP2035_V2021_scnC2035.xlsx
+++ b/src/egon/data/importing/nep_input_data/NEP2035_V2021_scnC2035.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Einheit</t>
   </si>
   <si>
-    <t xml:space="preserve">Baden-Wuerttemberg</t>
+    <t xml:space="preserve">Baden-Württemberg</t>
   </si>
   <si>
     <t xml:space="preserve">Bayern</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Schleswig-Holstein</t>
   </si>
   <si>
-    <t xml:space="preserve">Thueringen</t>
+    <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
     <t xml:space="preserve">Nordsee</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">KWK &lt; 10MW</t>
   </si>
   <si>
-    <t xml:space="preserve">Oesterreich</t>
+    <t xml:space="preserve">Österreich</t>
   </si>
   <si>
     <t xml:space="preserve">Luxemburg</t>
@@ -546,7 +546,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -559,7 +559,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.83"/>
@@ -568,7 +568,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.88"/>
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>